<commit_message>
Fixed IEC connectors mechanics, moved SD Card slot position
</commit_message>
<xml_diff>
--- a/Default Configuration/Outputs/BOM/BOM_PartType-REFLOW_CONTROLLER_V1_0.xlsx
+++ b/Default Configuration/Outputs/BOM/BOM_PartType-REFLOW_CONTROLLER_V1_0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98BBD2CB-6782-4A74-9F63-8DA9EDAF1331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A072F68-A4CE-4F64-844D-422A5F0AA4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18765" yWindow="4185" windowWidth="10035" windowHeight="11295" xr2:uid="{51823BD0-135A-4D7E-A6DC-B357B0D36BA2}"/>
+    <workbookView xWindow="18765" yWindow="4185" windowWidth="10035" windowHeight="11295" xr2:uid="{0414AB25-9D3E-424F-9EC0-799C909966F2}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-REFLOW_CONTROLLER_" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="253">
   <si>
     <t>Designator</t>
   </si>
@@ -770,6 +770,9 @@
   </si>
   <si>
     <t>U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512KB 1.7V~3.6V ARM-M4 128KB 180MHz FLASH 50 LQFP-64(10x10) Microcontrollers (MCU/MPU/SOC) ROHS  </t>
   </si>
   <si>
     <t>STMicroelectronics</t>
@@ -1167,7 +1170,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E65C82A8-8D01-4EE6-BDDD-72C0F6B29B5C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC97BEBC-F3AF-443A-94DA-CCEB9890A047}">
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -2317,25 +2320,25 @@
         <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>78</v>
+        <v>247</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>